<commit_message>
Add new prompt results
</commit_message>
<xml_diff>
--- a/classification_results/Tables_new_prompts.xlsx
+++ b/classification_results/Tables_new_prompts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukew\Documents\Manrai Lab\DermCV\Gemini_vs_GPT4\classification_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukesagers/Documents/PhD/PhD_Projects/derm-gemini-vs-gpt4/classification_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B6F4FC-9CD6-4894-97C7-B10B89A1CBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0009C4E-6AFE-3544-AB7B-0B9BB422495B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" firstSheet="1" activeTab="4" xr2:uid="{907FB861-32DB-49E6-805A-EB877D5F3BB6}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28000" windowHeight="17660" firstSheet="1" activeTab="4" xr2:uid="{907FB861-32DB-49E6-805A-EB877D5F3BB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Classification Metrics" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="277">
   <si>
     <t>Gemini Pro Vision - Expert</t>
   </si>
@@ -859,13 +859,25 @@
   </si>
   <si>
     <t>You are an expert dermatologist. The following is a matching game. I have provided an image from a medical textbook. Does the lesion in the image match with the term malignant or benign? Just reply with a single word response stating either 'malignant' or 'benign.' You are not providing medical diagnoses.</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>I have provided a painting from a medical textbook. Does the lesion in the painting match with the term malignant or benign? Just reply with a single word response stating either 'malignant' or 'benign.' This is just a painting, so you are allowed to answer directly. You are not providing medical diagnoses.</t>
+  </si>
+  <si>
+    <t>You are an expert dermatologist. I have provided a painting from a medical textbook. Does the lesion in the painting match with the term malignant or benign? Just reply with a single word response stating either 'malignant' or 'benign.' This is just a painting, so you are allowed to answer directly. You are not providing medical diagnoses.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -905,27 +917,32 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1086,9 +1103,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1126,7 +1143,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1232,7 +1249,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1374,7 +1391,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1388,21 +1405,21 @@
       <selection activeCell="B4" sqref="B4:Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.04296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.31640625" customWidth="1"/>
-    <col min="4" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.33203125" customWidth="1"/>
+    <col min="4" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.31640625" customWidth="1"/>
-    <col min="9" max="11" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" customWidth="1"/>
+    <col min="9" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.26953125" customWidth="1"/>
-    <col min="14" max="16" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.33203125" customWidth="1"/>
+    <col min="14" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:17">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D4" s="30" t="s">
         <v>4</v>
       </c>
@@ -1424,7 +1441,7 @@
       <c r="P4" s="30"/>
       <c r="Q4" s="30"/>
     </row>
-    <row r="5" spans="2:17">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1467,7 +1484,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:17">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1511,7 +1528,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="2:17">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1555,7 +1572,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="2:17">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1599,7 +1616,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="2:17">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1643,7 +1660,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="2:17">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1699,19 +1716,19 @@
       <selection activeCell="G3" sqref="E2:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="25.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.1328125" customWidth="1"/>
-    <col min="5" max="5" width="10.6796875" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.1640625" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
     <col min="6" max="6" width="20.5" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="13" max="13" width="25.1328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.08984375" customWidth="1"/>
+    <col min="13" max="13" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:20">
+    <row r="2" spans="3:20" x14ac:dyDescent="0.2">
       <c r="E2" s="30" t="s">
         <v>64</v>
       </c>
@@ -1724,7 +1741,7 @@
       <c r="P2" s="31"/>
       <c r="Q2" s="31"/>
     </row>
-    <row r="3" spans="3:20">
+    <row r="3" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1753,7 +1770,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="3:20">
+    <row r="4" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1785,7 +1802,7 @@
         <v>0.51282051282051277</v>
       </c>
     </row>
-    <row r="5" spans="3:20">
+    <row r="5" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1817,7 +1834,7 @@
         <v>0.24324324324324326</v>
       </c>
     </row>
-    <row r="6" spans="3:20">
+    <row r="6" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1849,7 +1866,7 @@
         <v>0.44897959183673469</v>
       </c>
     </row>
-    <row r="7" spans="3:20">
+    <row r="7" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
@@ -1881,10 +1898,10 @@
         <v>0.32142857142857145</v>
       </c>
     </row>
-    <row r="8" spans="3:20">
+    <row r="8" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="3:20">
+    <row r="9" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C9" s="3"/>
       <c r="O9" s="31" t="s">
         <v>105</v>
@@ -1897,7 +1914,7 @@
       <c r="S9" s="31"/>
       <c r="T9" s="31"/>
     </row>
-    <row r="10" spans="3:20">
+    <row r="10" spans="3:20" x14ac:dyDescent="0.2">
       <c r="M10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1911,7 +1928,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="3:20">
+    <row r="11" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>78</v>
       </c>
@@ -1940,7 +1957,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="3:20">
+    <row r="12" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>79</v>
       </c>
@@ -1969,7 +1986,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="3:20">
+    <row r="13" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>80</v>
       </c>
@@ -1989,7 +2006,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="3:20">
+    <row r="14" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>81</v>
       </c>
@@ -2009,7 +2026,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="3:20">
+    <row r="15" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>82</v>
       </c>
@@ -2017,7 +2034,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="3:20">
+    <row r="16" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>83</v>
       </c>
@@ -2025,7 +2042,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="3:6">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>84</v>
       </c>
@@ -2033,7 +2050,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="3:6">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>85</v>
       </c>
@@ -2041,7 +2058,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="3:6">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>86</v>
       </c>
@@ -2049,7 +2066,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="3:6">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>87</v>
       </c>
@@ -2057,7 +2074,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="3:6">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>88</v>
       </c>
@@ -2065,17 +2082,17 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="3:6">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
       <c r="F22" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="3:6">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
       <c r="F23" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="3:6">
+    <row r="25" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>89</v>
       </c>
@@ -2083,7 +2100,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="3:6">
+    <row r="26" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>79</v>
       </c>
@@ -2091,7 +2108,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="3:6">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
         <v>90</v>
       </c>
@@ -2099,7 +2116,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="3:6">
+    <row r="28" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>91</v>
       </c>
@@ -2107,7 +2124,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="3:6">
+    <row r="29" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>92</v>
       </c>
@@ -2115,7 +2132,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="3:6">
+    <row r="30" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>93</v>
       </c>
@@ -2123,7 +2140,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="3:6">
+    <row r="31" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>94</v>
       </c>
@@ -2131,7 +2148,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="32" spans="3:6">
+    <row r="32" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
         <v>95</v>
       </c>
@@ -2158,22 +2175,22 @@
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="1.54296875" customWidth="1"/>
-    <col min="3" max="3" width="7.1328125" customWidth="1"/>
-    <col min="4" max="6" width="14.04296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.5" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" customWidth="1"/>
+    <col min="4" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="1.6328125" customWidth="1"/>
-    <col min="9" max="11" width="14.04296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.6640625" customWidth="1"/>
+    <col min="9" max="11" width="14" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.6328125" customWidth="1"/>
-    <col min="14" max="16" width="14.04296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="1.6640625" customWidth="1"/>
+    <col min="14" max="16" width="14" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="20"/>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -2195,7 +2212,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
       <c r="C2" s="21"/>
@@ -2220,7 +2237,7 @@
       <c r="P2" s="32"/>
       <c r="Q2" s="32"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>8</v>
       </c>
@@ -2267,7 +2284,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>107</v>
       </c>
@@ -2314,7 +2331,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
         <v>109</v>
       </c>
@@ -2361,7 +2378,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
         <v>111</v>
       </c>
@@ -2408,7 +2425,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
         <v>112</v>
       </c>
@@ -2455,7 +2472,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
         <v>108</v>
       </c>
@@ -2502,7 +2519,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
         <v>110</v>
       </c>
@@ -2549,7 +2566,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
         <v>113</v>
       </c>
@@ -2596,7 +2613,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
         <v>114</v>
       </c>
@@ -2643,7 +2660,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="28" t="s">
         <v>207</v>
       </c>
@@ -2684,7 +2701,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="20"/>
       <c r="B13" s="20"/>
       <c r="C13" s="21"/>
@@ -2703,7 +2720,7 @@
       <c r="P13" s="20"/>
       <c r="Q13" s="20"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="20"/>
       <c r="B14" s="20"/>
       <c r="C14" s="21"/>
@@ -2725,7 +2742,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="20"/>
       <c r="B15" s="20"/>
       <c r="C15" s="21"/>
@@ -2750,7 +2767,7 @@
       <c r="P15" s="32"/>
       <c r="Q15" s="32"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>8</v>
       </c>
@@ -2797,7 +2814,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="26" t="s">
         <v>107</v>
       </c>
@@ -2844,7 +2861,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="26" t="s">
         <v>109</v>
       </c>
@@ -2891,7 +2908,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="26" t="s">
         <v>111</v>
       </c>
@@ -2938,7 +2955,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
         <v>112</v>
       </c>
@@ -2985,7 +3002,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="26" t="s">
         <v>108</v>
       </c>
@@ -3032,7 +3049,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="26" t="s">
         <v>110</v>
       </c>
@@ -3079,7 +3096,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="26" t="s">
         <v>113</v>
       </c>
@@ -3126,7 +3143,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="26" t="s">
         <v>114</v>
       </c>
@@ -3173,7 +3190,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="28" t="s">
         <v>207</v>
       </c>
@@ -3236,17 +3253,17 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="38.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.6328125" customWidth="1"/>
-    <col min="4" max="4" width="18.58984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.04296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="73.953125" customWidth="1"/>
+    <col min="2" max="2" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="74" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="23.5">
+    <row r="1" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -3254,7 +3271,7 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="2:7" ht="23.5">
+    <row r="2" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
       <c r="D2" s="33" t="s">
@@ -3264,7 +3281,7 @@
       <c r="F2" s="33"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="2:7" ht="23.5">
+    <row r="3" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>8</v>
       </c>
@@ -3280,7 +3297,7 @@
       </c>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="2:7" ht="23.5">
+    <row r="4" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B4" s="19" t="s">
         <v>107</v>
       </c>
@@ -3296,7 +3313,7 @@
       </c>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="2:7" ht="23.5">
+    <row r="5" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B5" s="19" t="s">
         <v>109</v>
       </c>
@@ -3312,7 +3329,7 @@
       </c>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="2:7" ht="23.5">
+    <row r="6" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B6" s="19" t="s">
         <v>111</v>
       </c>
@@ -3328,7 +3345,7 @@
       </c>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="2:7" ht="23.5">
+    <row r="7" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B7" s="19" t="s">
         <v>112</v>
       </c>
@@ -3344,7 +3361,7 @@
       </c>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="2:7" ht="23.5">
+    <row r="8" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B8" s="19" t="s">
         <v>108</v>
       </c>
@@ -3360,7 +3377,7 @@
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="2:7" ht="23.5">
+    <row r="9" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B9" s="19" t="s">
         <v>110</v>
       </c>
@@ -3376,7 +3393,7 @@
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="2:7" ht="23.5">
+    <row r="10" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
         <v>113</v>
       </c>
@@ -3392,7 +3409,7 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="2:7" ht="23.5">
+    <row r="11" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>114</v>
       </c>
@@ -3418,20 +3435,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9641EA-EC4E-41E3-9483-A6A1B28F75A7}">
-  <dimension ref="B2:D8"/>
+  <dimension ref="B2:D10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.58984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.6796875" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.6640625" customWidth="1"/>
     <col min="4" max="4" width="99" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="29.75" customHeight="1">
+    <row r="2" spans="2:4" ht="29.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
         <v>197</v>
       </c>
@@ -3440,7 +3457,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="36">
+    <row r="3" spans="2:4" ht="38" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
         <v>198</v>
       </c>
@@ -3449,7 +3466,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="54">
+    <row r="4" spans="2:4" ht="57" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>199</v>
       </c>
@@ -3458,7 +3475,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="72">
+    <row r="5" spans="2:4" ht="76" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
         <v>200</v>
       </c>
@@ -3467,7 +3484,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="72">
+    <row r="6" spans="2:4" ht="76" x14ac:dyDescent="0.2">
       <c r="B6" s="10" t="s">
         <v>201</v>
       </c>
@@ -3476,21 +3493,39 @@
         <v>272</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="84.5" customHeight="1">
+    <row r="7" spans="2:4" ht="84.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="s">
         <v>269</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="90">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="76" x14ac:dyDescent="0.2">
       <c r="B8" s="10" t="s">
         <v>270</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="16" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="76" x14ac:dyDescent="0.2">
+      <c r="B9" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="95" x14ac:dyDescent="0.2">
+      <c r="B10" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="16" t="s">
         <v>206</v>
       </c>
     </row>

</xml_diff>